<commit_message>
ensured StudentsT copula used degrees of freedom
</commit_message>
<xml_diff>
--- a/Copula_Based_Model.xlsx
+++ b/Copula_Based_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\james\IFOA_WG_Capital_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F8F459-AE68-41B9-B0F7-5E9A3E4284DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56467E08-312B-4889-9BFD-B154EDDCDBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="4275" windowWidth="33825" windowHeight="14535" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="4275" windowWidth="33825" windowHeight="14535" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Underwriting" sheetId="1" r:id="rId1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
   <si>
     <t>Poisson_Parameter</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>inflation_change</t>
+  </si>
+  <si>
+    <t>Class_DoF</t>
   </si>
 </sst>
 </file>
@@ -998,13 +1001,16 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3127CAE5-DDEB-4810-904E-F61DE554266B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1028,6 +1034,14 @@
       </c>
       <c r="B3">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2563,8 +2577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
removed large losses. simplified reserve risk calculation. updated parameters
</commit_message>
<xml_diff>
--- a/Copula_Based_Model.xlsx
+++ b/Copula_Based_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\james\IFOA_WG_Capital_Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56467E08-312B-4889-9BFD-B154EDDCDBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64A85EF-DC59-4AF3-BDDC-B024C626CF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="4275" windowWidth="33825" windowHeight="14535" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Underwriting" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -70,19 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="75">
-  <si>
-    <t>Poisson_Parameter</t>
-  </si>
-  <si>
-    <t>GDP_Shape_Parameter</t>
-  </si>
-  <si>
-    <t>GDP_Scale_Parameter</t>
-  </si>
-  <si>
-    <t>GDP_Loc_Parameter</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="73">
   <si>
     <t>Gamma_Alpha_Parameter</t>
   </si>
@@ -165,15 +153,9 @@
     <t>CAT_XoL_Retention</t>
   </si>
   <si>
-    <t>Large_XoL_Retention</t>
-  </si>
-  <si>
     <t>CAT_XoL_Limit</t>
   </si>
   <si>
-    <t>Large_XoL_Limit</t>
-  </si>
-  <si>
     <t>Losses_Aggregation_Theta</t>
   </si>
   <si>
@@ -295,16 +277,29 @@
   </si>
   <si>
     <t>Class_DoF</t>
+  </si>
+  <si>
+    <t>UW</t>
+  </si>
+  <si>
+    <t>Res</t>
+  </si>
+  <si>
+    <t>Mean LR</t>
+  </si>
+  <si>
+    <t>CoV LR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -344,7 +339,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -378,13 +373,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -401,11 +410,19 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="2" xr:uid="{F028AF62-25C6-4DB6-8767-2B034B3A6A19}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -864,134 +881,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>1887000000</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>0.4</v>
-      </c>
-      <c r="E2">
-        <v>21434272.127814323</v>
-      </c>
-      <c r="F2">
-        <v>6176213.1203094749</v>
-      </c>
-      <c r="G2">
-        <v>2.1665774084699665</v>
-      </c>
-      <c r="H2">
-        <v>387246722.29302722</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.67938021460906595</v>
+      </c>
+      <c r="E2" s="7">
+        <f>1/D2^2</f>
+        <v>2.1665774080000006</v>
+      </c>
+      <c r="F2" s="5">
+        <f>C2*B2/E2</f>
+        <v>435479478.60813278</v>
+      </c>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>3050000000</v>
       </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>0.4</v>
-      </c>
-      <c r="E3">
-        <v>12123239.056982597</v>
-      </c>
-      <c r="F3">
-        <v>47594601.571695596</v>
-      </c>
-      <c r="G3">
-        <v>6.9249013413173603</v>
-      </c>
-      <c r="H3">
-        <v>163179220.0779942</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0.38000840708731226</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E4" si="0">1/D3^2</f>
+        <v>6.9249013410000009</v>
+      </c>
+      <c r="F3" s="5">
+        <f>C3*B3/E3</f>
+        <v>264263692.70637667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>1887000000</v>
       </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>0.4</v>
-      </c>
-      <c r="E4">
-        <v>10012524.013125015</v>
-      </c>
-      <c r="F4">
-        <v>39212459.978124946</v>
-      </c>
-      <c r="G4">
-        <v>6.9243640207395618</v>
-      </c>
-      <c r="H4">
-        <v>111057130.6888963</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G8" s="5"/>
+      <c r="C4" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.38002315083530841</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>6.9243640209999997</v>
+      </c>
+      <c r="F4" s="5">
+        <f>C4*B4/E4</f>
+        <v>190761201.46110383</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="14"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="14"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="14"/>
+      <c r="C8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1003,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3127CAE5-DDEB-4810-904E-F61DE554266B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1014,15 +1020,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>1.2</v>
@@ -1030,7 +1036,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>1.5</v>
@@ -1038,7 +1044,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1054,7 +1060,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,26 +1070,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B2">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1109,10 +1115,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1364,7 +1370,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1374,16 +1380,16 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1779,8 +1785,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,48 +1798,48 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>5000000000</v>
+        <v>2000000000</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
         <v>1000000000</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
-        <v>8000000000</v>
+        <v>4000000000</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0.15</v>
       </c>
       <c r="G4" s="4"/>
     </row>
@@ -1847,7 +1853,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C18"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1859,21 +1865,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
@@ -1881,10 +1887,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C3" s="7">
         <v>0.02</v>
@@ -1892,10 +1898,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" s="7">
         <v>0.02</v>
@@ -1903,10 +1909,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C5" s="7">
         <v>0</v>
@@ -1914,10 +1920,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C6" s="7">
         <v>0.1</v>
@@ -1925,10 +1931,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" s="7">
         <v>0.25</v>
@@ -1936,10 +1942,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C8" s="7">
         <v>0</v>
@@ -1947,10 +1953,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C9" s="7">
         <v>0.1</v>
@@ -1958,10 +1964,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C10" s="9">
         <v>14000000000</v>
@@ -1969,10 +1975,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C11" s="7">
         <v>0.5</v>
@@ -1980,10 +1986,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C12" s="7">
         <v>0.02</v>
@@ -1991,10 +1997,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C13" s="7">
         <v>-2</v>
@@ -2002,10 +2008,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C14" s="7">
         <v>0.2</v>
@@ -2013,10 +2019,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15" s="7">
         <v>0.5</v>
@@ -2024,10 +2030,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C16" s="7">
         <v>-1</v>
@@ -2035,10 +2041,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C17" s="7">
         <v>0</v>
@@ -2046,10 +2052,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C18" s="7">
         <v>0.03</v>
@@ -2088,15 +2094,15 @@
         <v>credit_spread</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2104,7 +2110,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>-0.2</v>
@@ -2115,7 +2121,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>0.2</v>
@@ -2129,7 +2135,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>-0.3</v>
@@ -2146,7 +2152,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B6">
         <v>0.2</v>
@@ -2166,7 +2172,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B7">
         <v>0.5</v>
@@ -2197,7 +2203,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,21 +2214,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>0.01</v>
@@ -2230,10 +2236,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>0.05</v>
@@ -2241,10 +2247,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
       </c>
       <c r="C4">
         <v>0.1</v>
@@ -2252,10 +2258,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -2263,10 +2269,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2274,10 +2280,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C7">
         <v>1.5</v>
@@ -2285,120 +2291,120 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>54</v>
       </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C18">
         <v>0.1</v>
@@ -2406,10 +2412,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <v>0.1</v>
@@ -2417,10 +2423,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>0.1</v>
@@ -2428,10 +2434,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C21">
         <v>0.1</v>
@@ -2439,10 +2445,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C22">
         <v>0.1</v>
@@ -2450,10 +2456,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C23">
         <v>0.1</v>
@@ -2461,10 +2467,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C24">
         <v>0.1</v>
@@ -2472,10 +2478,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C25">
         <v>0.1</v>
@@ -2483,10 +2489,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C26">
         <v>0.1</v>
@@ -2494,10 +2500,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C27">
         <v>0.1</v>
@@ -2525,21 +2531,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2547,10 +2553,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -2559,10 +2565,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -2575,72 +2581,44 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>0.25</v>
       </c>
-      <c r="C2" s="4">
-        <v>10000000</v>
-      </c>
-      <c r="D2" s="4">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>0.25</v>
       </c>
-      <c r="C3" s="4">
-        <v>10000000</v>
-      </c>
-      <c r="D3" s="4">
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0.3</v>
-      </c>
-      <c r="C4" s="4">
-        <v>10000000</v>
-      </c>
-      <c r="D4" s="4">
-        <v>100000000</v>
       </c>
     </row>
   </sheetData>
@@ -2665,19 +2643,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4">
         <v>100000000</v>
@@ -2689,7 +2667,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B3" s="4">
         <v>500000000</v>
@@ -2700,7 +2678,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4">
         <v>300000000</v>
@@ -2711,7 +2689,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B5" s="4">
         <v>1000000000</v>
@@ -2727,65 +2705,209 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50CD9001-998B-4E20-AD63-7CEFD92BA227}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="7"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="str" cm="1">
-        <f t="array" ref="B1:D1">TRANSPOSE(A2:A4)</f>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="7" t="str">
+        <f t="array" ref="C2:H2">TRANSPOSE(B3:B8)</f>
         <v>Specialty</v>
       </c>
-      <c r="C1" t="str">
+      <c r="D2" s="7" t="str">
         <v>Property</v>
       </c>
-      <c r="D1" t="str">
+      <c r="E2" s="7" t="str">
         <v>Liability</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0.35</v>
-      </c>
-      <c r="D2">
-        <v>0.54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2" s="7" t="str">
+        <v>Specialty</v>
+      </c>
+      <c r="G2" s="7" t="str">
+        <v>Property</v>
+      </c>
+      <c r="H2" s="7" t="str">
+        <v>Liability</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>0.35</v>
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
+        <v>0.35</v>
+      </c>
+      <c r="E3">
+        <v>0.54</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="H3" s="7">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>0.35</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
+      <c r="F4" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
         <v>0.54</v>
       </c>
-      <c r="C4">
+      <c r="D5">
         <v>0.48</v>
       </c>
-      <c r="D4">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="D6">
+        <v>0.2</v>
+      </c>
+      <c r="E6">
+        <v>0.3</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="H6" s="7">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>0.2</v>
+      </c>
+      <c r="D7">
+        <v>0.4</v>
+      </c>
+      <c r="E7">
+        <v>0.3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0.35</v>
+      </c>
+      <c r="G7" s="7">
+        <v>1</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0.3</v>
+      </c>
+      <c r="D8">
+        <v>0.3</v>
+      </c>
+      <c r="E8">
+        <v>0.7</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0.54</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0.48</v>
+      </c>
+      <c r="H8" s="7">
         <v>1</v>
       </c>
     </row>

</xml_diff>